<commit_message>
notes excel file added
</commit_message>
<xml_diff>
--- a/notes-Meteor Todos.xlsx
+++ b/notes-Meteor Todos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Objective</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Have Multiple Status, Not Started, In Process, Completed</t>
+  </si>
+  <si>
+    <t>Use a color highlighter for the user name</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,8 +644,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>

</xml_diff>